<commit_message>
updated usage notes for destination arrays
</commit_message>
<xml_diff>
--- a/data dictionaries/Australian National Liveability Study 2018 - Data Dictionaries.xlsx
+++ b/data dictionaries/Australian National Liveability Study 2018 - Data Dictionaries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b6e883cba6f6f254/Research/Publications/Australian National Liveability Dataset 2018/data dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2131" documentId="8_{8927F8F2-8591-4312-826B-399B1EF6B5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F461D51E-EB23-4D04-85E4-570BC7B836D8}"/>
+  <xr:revisionPtr revIDLastSave="2132" documentId="8_{8927F8F2-8591-4312-826B-399B1EF6B5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C747745A-64F9-4AB9-896F-3C81B0216573}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{55DEBD08-1F64-4162-9001-EC2B420C9CEE}"/>
   </bookViews>
@@ -2625,9 +2625,6 @@
     <t>Format</t>
   </si>
   <si>
-    <t>11.6 Gb</t>
-  </si>
-  <si>
     <t>427 Mb</t>
   </si>
   <si>
@@ -3464,6 +3461,9 @@
   </si>
   <si>
     <t>TransPerth</t>
+  </si>
+  <si>
+    <t>11.2 Gb</t>
   </si>
 </sst>
 </file>
@@ -3636,7 +3636,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3818,6 +3818,48 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3836,62 +3878,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4211,7 +4202,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4237,17 +4230,17 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="81" t="s">
         <v>619</v>
       </c>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>856</v>
@@ -4259,271 +4252,271 @@
         <v>857</v>
       </c>
       <c r="E7" s="45" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B8" s="35">
         <v>6536400</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D8" s="36" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="E8" s="46" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="27" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B9" s="37">
         <v>6536400</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D9" s="38" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="E9" s="47" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B10" s="37">
         <v>6536400</v>
       </c>
       <c r="C10" s="38" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>859</v>
+        <v>1040</v>
       </c>
       <c r="E10" s="47" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B11" s="37">
         <v>183075</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="E11" s="47" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="29" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="B12" s="42">
         <v>39966</v>
       </c>
       <c r="C12" s="39" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D12" s="39" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="E12" s="47" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="29" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B13" s="42">
         <v>1498</v>
       </c>
       <c r="C13" s="39" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D13" s="39" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="E13" s="48" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="29" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B14" s="42">
         <v>223</v>
       </c>
       <c r="C14" s="39" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="E14" s="48" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="29" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B15" s="42">
         <v>63</v>
       </c>
       <c r="C15" s="39" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D15" s="39" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="E15" s="48" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="29" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B16" s="42">
         <v>3101</v>
       </c>
       <c r="C16" s="39" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D16" s="39" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="E16" s="48" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="29" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B17" s="42">
         <v>170</v>
       </c>
       <c r="C17" s="39" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="E17" s="48" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B18" s="42">
         <v>21</v>
       </c>
       <c r="C18" s="39" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D18" s="39" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="E18" s="48" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="29" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="B19" s="41">
         <v>111593</v>
       </c>
       <c r="C19" s="39" t="s">
+        <v>860</v>
+      </c>
+      <c r="D19" s="39" t="s">
         <v>861</v>
       </c>
-      <c r="D19" s="39" t="s">
-        <v>862</v>
-      </c>
       <c r="E19" s="48" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="29" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="B20" s="41">
         <v>69891</v>
       </c>
       <c r="C20" s="39" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D20" s="39" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="E20" s="48" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B21" s="43">
         <v>6535982</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="D21" s="40" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="E21" s="51" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B23" s="66"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
   </sheetData>
@@ -4576,7 +4569,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -6359,7 +6352,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -7336,7 +7329,7 @@
         <v>28</v>
       </c>
       <c r="D67" s="19" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="E67" s="15" t="s">
         <v>3</v>
@@ -7396,7 +7389,7 @@
         <v>32</v>
       </c>
       <c r="D71" s="19" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="E71" s="15" t="s">
         <v>3</v>
@@ -7952,17 +7945,17 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="82" t="s">
         <v>622</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -9630,13 +9623,13 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="83" t="s">
         <v>621</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -10813,81 +10806,81 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="84" t="s">
         <v>896</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="70" t="s">
+      <c r="B10" s="84"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="85" t="s">
         <v>897</v>
       </c>
-      <c r="B10" s="70"/>
-      <c r="C10" s="70"/>
-      <c r="D10" s="70"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="71" t="s">
-        <v>898</v>
-      </c>
-      <c r="B11" s="71"/>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="85"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="72"/>
-      <c r="B12" s="72"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="72"/>
+      <c r="A12" s="86"/>
+      <c r="B12" s="86"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="8" t="s">
@@ -10900,7 +10893,7 @@
         <v>538</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -10919,14 +10912,14 @@
         <v>8</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="13">
         <v>2</v>
       </c>
-      <c r="B15" s="73">
+      <c r="B15" s="67">
         <v>1</v>
       </c>
       <c r="C15" s="13"/>
@@ -10940,7 +10933,7 @@
         <v>8</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -10959,7 +10952,7 @@
         <v>8</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -10980,7 +10973,7 @@
         <v>8</v>
       </c>
       <c r="G17" s="19" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -11001,7 +10994,7 @@
         <v>8</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -11022,7 +11015,7 @@
         <v>8</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -11043,7 +11036,7 @@
         <v>8</v>
       </c>
       <c r="G20" s="19" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -11062,7 +11055,7 @@
         <v>8</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -11081,7 +11074,7 @@
         <v>8</v>
       </c>
       <c r="G22" s="19" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -11102,7 +11095,7 @@
         <v>8</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -11123,7 +11116,7 @@
         <v>8</v>
       </c>
       <c r="G24" s="19" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -11142,7 +11135,7 @@
         <v>8</v>
       </c>
       <c r="G25" s="19" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -11161,7 +11154,7 @@
         <v>8</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -11179,10 +11172,10 @@
         <v>553</v>
       </c>
       <c r="F27" s="19" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="G27" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -11200,10 +11193,10 @@
         <v>552</v>
       </c>
       <c r="F28" s="19" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="G28" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -11221,10 +11214,10 @@
         <v>555</v>
       </c>
       <c r="F29" s="19" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="G29" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -11242,10 +11235,10 @@
         <v>556</v>
       </c>
       <c r="F30" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G30" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -11263,10 +11256,10 @@
         <v>554</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -11284,10 +11277,10 @@
         <v>557</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G32" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -11297,16 +11290,16 @@
       </c>
       <c r="C33" s="13"/>
       <c r="D33" s="14" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="F33" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G33" s="19" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -11316,16 +11309,16 @@
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="14" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G34" s="19" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -11335,16 +11328,16 @@
       </c>
       <c r="C35" s="13"/>
       <c r="D35" s="14" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="E35" s="19" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="F35" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G35" s="19" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -11362,10 +11355,10 @@
         <v>629</v>
       </c>
       <c r="F36" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G36" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="37" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
@@ -11383,10 +11376,10 @@
         <v>630</v>
       </c>
       <c r="F37" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G37" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -11404,10 +11397,10 @@
         <v>310</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G38" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -11425,10 +11418,10 @@
         <v>312</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G39" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -11446,10 +11439,10 @@
         <v>314</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G40" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -11467,10 +11460,10 @@
         <v>316</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G41" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -11488,10 +11481,10 @@
         <v>318</v>
       </c>
       <c r="F42" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G42" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -11509,10 +11502,10 @@
         <v>320</v>
       </c>
       <c r="F43" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G43" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -11530,10 +11523,10 @@
         <v>322</v>
       </c>
       <c r="F44" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G44" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -11551,10 +11544,10 @@
         <v>197</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G45" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -11572,10 +11565,10 @@
         <v>210</v>
       </c>
       <c r="F46" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G46" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -11593,10 +11586,10 @@
         <v>186</v>
       </c>
       <c r="F47" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G47" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -11614,10 +11607,10 @@
         <v>184</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G48" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -11635,10 +11628,10 @@
         <v>251</v>
       </c>
       <c r="F49" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G49" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -11656,10 +11649,10 @@
         <v>255</v>
       </c>
       <c r="F50" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G50" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -11677,10 +11670,10 @@
         <v>631</v>
       </c>
       <c r="F51" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G51" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -11698,10 +11691,10 @@
         <v>632</v>
       </c>
       <c r="F52" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G52" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -11719,10 +11712,10 @@
         <v>187</v>
       </c>
       <c r="F53" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G53" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -11740,10 +11733,10 @@
         <v>264</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G54" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -11761,10 +11754,10 @@
         <v>172</v>
       </c>
       <c r="F55" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G55" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -11782,10 +11775,10 @@
         <v>173</v>
       </c>
       <c r="F56" s="19" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G56" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -11795,16 +11788,16 @@
       </c>
       <c r="C57" s="13"/>
       <c r="D57" s="14" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="E57" s="19" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="F57" s="19" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -11814,16 +11807,16 @@
       </c>
       <c r="C58" s="13"/>
       <c r="D58" s="14" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="E58" s="19" t="s">
+        <v>989</v>
+      </c>
+      <c r="F58" s="19" t="s">
+        <v>960</v>
+      </c>
+      <c r="G58" s="19" t="s">
         <v>990</v>
-      </c>
-      <c r="F58" s="19" t="s">
-        <v>961</v>
-      </c>
-      <c r="G58" s="19" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -11841,10 +11834,10 @@
         <v>175</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G59" s="15" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -11862,10 +11855,10 @@
         <v>176</v>
       </c>
       <c r="F60" s="15" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G60" s="15" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -11883,10 +11876,10 @@
         <v>178</v>
       </c>
       <c r="F61" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G61" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -11904,10 +11897,10 @@
         <v>855</v>
       </c>
       <c r="F62" s="19" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G62" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -11925,10 +11918,10 @@
         <v>853</v>
       </c>
       <c r="F63" s="19" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G63" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -11946,10 +11939,10 @@
         <v>854</v>
       </c>
       <c r="F64" s="19" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G64" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -11967,10 +11960,10 @@
         <v>180</v>
       </c>
       <c r="F65" s="15" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G65" s="15" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -11988,10 +11981,10 @@
         <v>182</v>
       </c>
       <c r="F66" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G66" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -12009,10 +12002,10 @@
         <v>558</v>
       </c>
       <c r="F67" s="15" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G67" s="15" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12030,10 +12023,10 @@
         <v>190</v>
       </c>
       <c r="F68" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G68" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12051,10 +12044,10 @@
         <v>191</v>
       </c>
       <c r="F69" s="19" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G69" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -12072,10 +12065,10 @@
         <v>192</v>
       </c>
       <c r="F70" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G70" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -12093,10 +12086,10 @@
         <v>193</v>
       </c>
       <c r="F71" s="19" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G71" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12114,10 +12107,10 @@
         <v>194</v>
       </c>
       <c r="F72" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G72" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12135,10 +12128,10 @@
         <v>195</v>
       </c>
       <c r="F73" s="19" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G73" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -12156,10 +12149,10 @@
         <v>200</v>
       </c>
       <c r="F74" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G74" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -12177,10 +12170,10 @@
         <v>201</v>
       </c>
       <c r="F75" s="19" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G75" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12198,10 +12191,10 @@
         <v>202</v>
       </c>
       <c r="F76" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G76" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12219,10 +12212,10 @@
         <v>203</v>
       </c>
       <c r="F77" s="19" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G77" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -12240,10 +12233,10 @@
         <v>204</v>
       </c>
       <c r="F78" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G78" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12261,10 +12254,10 @@
         <v>197</v>
       </c>
       <c r="F79" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G79" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12282,10 +12275,10 @@
         <v>206</v>
       </c>
       <c r="F80" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G80" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12303,10 +12296,10 @@
         <v>208</v>
       </c>
       <c r="F81" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G81" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -12324,10 +12317,10 @@
         <v>209</v>
       </c>
       <c r="F82" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G82" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -12345,10 +12338,10 @@
         <v>210</v>
       </c>
       <c r="F83" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G83" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -12366,10 +12359,10 @@
         <v>209</v>
       </c>
       <c r="F84" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G84" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -12387,10 +12380,10 @@
         <v>211</v>
       </c>
       <c r="F85" s="19" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G85" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -12408,10 +12401,10 @@
         <v>212</v>
       </c>
       <c r="F86" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G86" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -12429,10 +12422,10 @@
         <v>213</v>
       </c>
       <c r="F87" s="19" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G87" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -12450,10 +12443,10 @@
         <v>214</v>
       </c>
       <c r="F88" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G88" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -12471,10 +12464,10 @@
         <v>215</v>
       </c>
       <c r="F89" s="19" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G89" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12492,10 +12485,10 @@
         <v>216</v>
       </c>
       <c r="F90" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G90" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12513,10 +12506,10 @@
         <v>217</v>
       </c>
       <c r="F91" s="19" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G91" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -12534,10 +12527,10 @@
         <v>218</v>
       </c>
       <c r="F92" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G92" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -12555,10 +12548,10 @@
         <v>219</v>
       </c>
       <c r="F93" s="19" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G93" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12576,10 +12569,10 @@
         <v>220</v>
       </c>
       <c r="F94" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G94" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12597,10 +12590,10 @@
         <v>221</v>
       </c>
       <c r="F95" s="19" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G95" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -12618,10 +12611,10 @@
         <v>222</v>
       </c>
       <c r="F96" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G96" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -12639,10 +12632,10 @@
         <v>223</v>
       </c>
       <c r="F97" s="19" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G97" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -12660,10 +12653,10 @@
         <v>224</v>
       </c>
       <c r="F98" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G98" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -12681,10 +12674,10 @@
         <v>225</v>
       </c>
       <c r="F99" s="19" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G99" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -12702,10 +12695,10 @@
         <v>226</v>
       </c>
       <c r="F100" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G100" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -12723,10 +12716,10 @@
         <v>227</v>
       </c>
       <c r="F101" s="19" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="G101" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -12744,10 +12737,10 @@
         <v>229</v>
       </c>
       <c r="F102" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G102" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -12765,10 +12758,10 @@
         <v>230</v>
       </c>
       <c r="F103" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G103" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -12786,10 +12779,10 @@
         <v>232</v>
       </c>
       <c r="F104" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G104" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -12807,10 +12800,10 @@
         <v>234</v>
       </c>
       <c r="F105" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G105" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -12828,10 +12821,10 @@
         <v>236</v>
       </c>
       <c r="F106" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G106" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -12846,13 +12839,13 @@
         <v>32</v>
       </c>
       <c r="E107" s="19" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="F107" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G107" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -12870,10 +12863,10 @@
         <v>238</v>
       </c>
       <c r="F108" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G108" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12891,10 +12884,10 @@
         <v>240</v>
       </c>
       <c r="F109" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G109" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -12912,10 +12905,10 @@
         <v>242</v>
       </c>
       <c r="F110" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G110" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12933,10 +12926,10 @@
         <v>244</v>
       </c>
       <c r="F111" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G111" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -12954,10 +12947,10 @@
         <v>246</v>
       </c>
       <c r="F112" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G112" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -12975,10 +12968,10 @@
         <v>248</v>
       </c>
       <c r="F113" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G113" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -12996,10 +12989,10 @@
         <v>250</v>
       </c>
       <c r="F114" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G114" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -13017,10 +13010,10 @@
         <v>253</v>
       </c>
       <c r="F115" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G115" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -13038,10 +13031,10 @@
         <v>257</v>
       </c>
       <c r="F116" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G116" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -13059,10 +13052,10 @@
         <v>259</v>
       </c>
       <c r="F117" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G117" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -13080,10 +13073,10 @@
         <v>261</v>
       </c>
       <c r="F118" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G118" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -13101,10 +13094,10 @@
         <v>266</v>
       </c>
       <c r="F119" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G119" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -13122,10 +13115,10 @@
         <v>268</v>
       </c>
       <c r="F120" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G120" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -13143,10 +13136,10 @@
         <v>270</v>
       </c>
       <c r="F121" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G121" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="122" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -13164,10 +13157,10 @@
         <v>272</v>
       </c>
       <c r="F122" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G122" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -13185,10 +13178,10 @@
         <v>274</v>
       </c>
       <c r="F123" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G123" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -13206,10 +13199,10 @@
         <v>276</v>
       </c>
       <c r="F124" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G124" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="125" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -13227,10 +13220,10 @@
         <v>278</v>
       </c>
       <c r="F125" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G125" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -13248,10 +13241,10 @@
         <v>280</v>
       </c>
       <c r="F126" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G126" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -13269,10 +13262,10 @@
         <v>282</v>
       </c>
       <c r="F127" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G127" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -13290,10 +13283,10 @@
         <v>284</v>
       </c>
       <c r="F128" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G128" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -13311,10 +13304,10 @@
         <v>286</v>
       </c>
       <c r="F129" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G129" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -13332,10 +13325,10 @@
         <v>188</v>
       </c>
       <c r="F130" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G130" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="131" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -13353,10 +13346,10 @@
         <v>288</v>
       </c>
       <c r="F131" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G131" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -13374,10 +13367,10 @@
         <v>290</v>
       </c>
       <c r="F132" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G132" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -13395,10 +13388,10 @@
         <v>292</v>
       </c>
       <c r="F133" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G133" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
@@ -13416,10 +13409,10 @@
         <v>294</v>
       </c>
       <c r="F134" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G134" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
@@ -13437,10 +13430,10 @@
         <v>296</v>
       </c>
       <c r="F135" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G135" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -13458,10 +13451,10 @@
         <v>298</v>
       </c>
       <c r="F136" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G136" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
@@ -13479,10 +13472,10 @@
         <v>300</v>
       </c>
       <c r="F137" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G137" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
@@ -13500,10 +13493,10 @@
         <v>302</v>
       </c>
       <c r="F138" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G138" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
@@ -13521,10 +13514,10 @@
         <v>304</v>
       </c>
       <c r="F139" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G139" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
@@ -13542,10 +13535,10 @@
         <v>306</v>
       </c>
       <c r="F140" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G140" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -13563,10 +13556,10 @@
         <v>308</v>
       </c>
       <c r="F141" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G141" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
@@ -13584,10 +13577,10 @@
         <v>199</v>
       </c>
       <c r="F142" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G142" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
@@ -13605,10 +13598,10 @@
         <v>447</v>
       </c>
       <c r="F143" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G143" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
@@ -13626,10 +13619,10 @@
         <v>324</v>
       </c>
       <c r="F144" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G144" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
@@ -13647,10 +13640,10 @@
         <v>326</v>
       </c>
       <c r="F145" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G145" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
@@ -13668,10 +13661,10 @@
         <v>328</v>
       </c>
       <c r="F146" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G146" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
@@ -13689,10 +13682,10 @@
         <v>380</v>
       </c>
       <c r="F147" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G147" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
@@ -13710,10 +13703,10 @@
         <v>332</v>
       </c>
       <c r="F148" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G148" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
@@ -13731,10 +13724,10 @@
         <v>334</v>
       </c>
       <c r="F149" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G149" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
@@ -13752,10 +13745,10 @@
         <v>378</v>
       </c>
       <c r="F150" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G150" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
@@ -13773,10 +13766,10 @@
         <v>330</v>
       </c>
       <c r="F151" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G151" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
@@ -13794,10 +13787,10 @@
         <v>426</v>
       </c>
       <c r="F152" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G152" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
@@ -13815,10 +13808,10 @@
         <v>358</v>
       </c>
       <c r="F153" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G153" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
@@ -13836,10 +13829,10 @@
         <v>360</v>
       </c>
       <c r="F154" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G154" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
@@ -13857,10 +13850,10 @@
         <v>362</v>
       </c>
       <c r="F155" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G155" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
@@ -13878,10 +13871,10 @@
         <v>364</v>
       </c>
       <c r="F156" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G156" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="157" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -13899,10 +13892,10 @@
         <v>366</v>
       </c>
       <c r="F157" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G157" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="158" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -13920,10 +13913,10 @@
         <v>368</v>
       </c>
       <c r="F158" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G158" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
@@ -13941,10 +13934,10 @@
         <v>370</v>
       </c>
       <c r="F159" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G159" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
@@ -13962,10 +13955,10 @@
         <v>372</v>
       </c>
       <c r="F160" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G160" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -13983,10 +13976,10 @@
         <v>374</v>
       </c>
       <c r="F161" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G161" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
@@ -14004,10 +13997,10 @@
         <v>336</v>
       </c>
       <c r="F162" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G162" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
@@ -14025,10 +14018,10 @@
         <v>338</v>
       </c>
       <c r="F163" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G163" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -14046,10 +14039,10 @@
         <v>350</v>
       </c>
       <c r="F164" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G164" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
@@ -14067,10 +14060,10 @@
         <v>408</v>
       </c>
       <c r="F165" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G165" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
@@ -14088,10 +14081,10 @@
         <v>449</v>
       </c>
       <c r="F166" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G166" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
@@ -14109,10 +14102,10 @@
         <v>410</v>
       </c>
       <c r="F167" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G167" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
@@ -14130,10 +14123,10 @@
         <v>412</v>
       </c>
       <c r="F168" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G168" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
@@ -14151,10 +14144,10 @@
         <v>428</v>
       </c>
       <c r="F169" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G169" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
@@ -14172,10 +14165,10 @@
         <v>414</v>
       </c>
       <c r="F170" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G170" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
@@ -14193,10 +14186,10 @@
         <v>416</v>
       </c>
       <c r="F171" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G171" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
@@ -14214,10 +14207,10 @@
         <v>418</v>
       </c>
       <c r="F172" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G172" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
@@ -14235,10 +14228,10 @@
         <v>451</v>
       </c>
       <c r="F173" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G173" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
@@ -14256,10 +14249,10 @@
         <v>453</v>
       </c>
       <c r="F174" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G174" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
@@ -14277,10 +14270,10 @@
         <v>455</v>
       </c>
       <c r="F175" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G175" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
@@ -14298,10 +14291,10 @@
         <v>457</v>
       </c>
       <c r="F176" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G176" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
@@ -14319,10 +14312,10 @@
         <v>459</v>
       </c>
       <c r="F177" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G177" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
@@ -14340,10 +14333,10 @@
         <v>461</v>
       </c>
       <c r="F178" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G178" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="179" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -14361,10 +14354,10 @@
         <v>463</v>
       </c>
       <c r="F179" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G179" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="180" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -14382,10 +14375,10 @@
         <v>465</v>
       </c>
       <c r="F180" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G180" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="181" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -14403,10 +14396,10 @@
         <v>467</v>
       </c>
       <c r="F181" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G181" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
@@ -14424,10 +14417,10 @@
         <v>455</v>
       </c>
       <c r="F182" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G182" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="183" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -14445,10 +14438,10 @@
         <v>469</v>
       </c>
       <c r="F183" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G183" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="184" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -14466,10 +14459,10 @@
         <v>471</v>
       </c>
       <c r="F184" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G184" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="185" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -14487,10 +14480,10 @@
         <v>473</v>
       </c>
       <c r="F185" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G185" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
@@ -14508,10 +14501,10 @@
         <v>475</v>
       </c>
       <c r="F186" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G186" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
@@ -14529,10 +14522,10 @@
         <v>453</v>
       </c>
       <c r="F187" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G187" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="188" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -14550,10 +14543,10 @@
         <v>497</v>
       </c>
       <c r="F188" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G188" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="189" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -14571,10 +14564,10 @@
         <v>477</v>
       </c>
       <c r="F189" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G189" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="190" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -14592,10 +14585,10 @@
         <v>479</v>
       </c>
       <c r="F190" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G190" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="191" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -14613,10 +14606,10 @@
         <v>481</v>
       </c>
       <c r="F191" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G191" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
@@ -14634,10 +14627,10 @@
         <v>483</v>
       </c>
       <c r="F192" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G192" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="193" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -14655,10 +14648,10 @@
         <v>485</v>
       </c>
       <c r="F193" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G193" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="194" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -14676,10 +14669,10 @@
         <v>487</v>
       </c>
       <c r="F194" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G194" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="195" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -14697,10 +14690,10 @@
         <v>489</v>
       </c>
       <c r="F195" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G195" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
@@ -14718,10 +14711,10 @@
         <v>461</v>
       </c>
       <c r="F196" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G196" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
@@ -14739,10 +14732,10 @@
         <v>493</v>
       </c>
       <c r="F197" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G197" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
@@ -14760,10 +14753,10 @@
         <v>340</v>
       </c>
       <c r="F198" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G198" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
@@ -14781,10 +14774,10 @@
         <v>356</v>
       </c>
       <c r="F199" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G199" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
@@ -14802,10 +14795,10 @@
         <v>420</v>
       </c>
       <c r="F200" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G200" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
@@ -14823,10 +14816,10 @@
         <v>342</v>
       </c>
       <c r="F201" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G201" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
@@ -14844,10 +14837,10 @@
         <v>352</v>
       </c>
       <c r="F202" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G202" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
@@ -14865,10 +14858,10 @@
         <v>436</v>
       </c>
       <c r="F203" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G203" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
@@ -14886,10 +14879,10 @@
         <v>442</v>
       </c>
       <c r="F204" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G204" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
@@ -14907,10 +14900,10 @@
         <v>444</v>
       </c>
       <c r="F205" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G205" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
@@ -14928,10 +14921,10 @@
         <v>446</v>
       </c>
       <c r="F206" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G206" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
@@ -14949,10 +14942,10 @@
         <v>438</v>
       </c>
       <c r="F207" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G207" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="208" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -14970,10 +14963,10 @@
         <v>491</v>
       </c>
       <c r="F208" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G208" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
@@ -14991,10 +14984,10 @@
         <v>440</v>
       </c>
       <c r="F209" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G209" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
@@ -15012,10 +15005,10 @@
         <v>382</v>
       </c>
       <c r="F210" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G210" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
@@ -15033,10 +15026,10 @@
         <v>384</v>
       </c>
       <c r="F211" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G211" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
@@ -15054,10 +15047,10 @@
         <v>386</v>
       </c>
       <c r="F212" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G212" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
@@ -15075,10 +15068,10 @@
         <v>388</v>
       </c>
       <c r="F213" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G213" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
@@ -15096,10 +15089,10 @@
         <v>354</v>
       </c>
       <c r="F214" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G214" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
@@ -15117,10 +15110,10 @@
         <v>434</v>
       </c>
       <c r="F215" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G215" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
@@ -15138,10 +15131,10 @@
         <v>344</v>
       </c>
       <c r="F216" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G216" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
@@ -15159,10 +15152,10 @@
         <v>376</v>
       </c>
       <c r="F217" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G217" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
@@ -15180,10 +15173,10 @@
         <v>346</v>
       </c>
       <c r="F218" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G218" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
@@ -15201,10 +15194,10 @@
         <v>390</v>
       </c>
       <c r="F219" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G219" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
@@ -15222,10 +15215,10 @@
         <v>392</v>
       </c>
       <c r="F220" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G220" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
@@ -15243,10 +15236,10 @@
         <v>394</v>
       </c>
       <c r="F221" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G221" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
@@ -15264,10 +15257,10 @@
         <v>396</v>
       </c>
       <c r="F222" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G222" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
@@ -15285,10 +15278,10 @@
         <v>430</v>
       </c>
       <c r="F223" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G223" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
@@ -15306,10 +15299,10 @@
         <v>495</v>
       </c>
       <c r="F224" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G224" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
@@ -15327,10 +15320,10 @@
         <v>432</v>
       </c>
       <c r="F225" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G225" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
@@ -15348,10 +15341,10 @@
         <v>398</v>
       </c>
       <c r="F226" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G226" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
@@ -15369,10 +15362,10 @@
         <v>400</v>
       </c>
       <c r="F227" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G227" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
@@ -15390,10 +15383,10 @@
         <v>402</v>
       </c>
       <c r="F228" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G228" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
@@ -15411,10 +15404,10 @@
         <v>404</v>
       </c>
       <c r="F229" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G229" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
@@ -15432,10 +15425,10 @@
         <v>406</v>
       </c>
       <c r="F230" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G230" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
@@ -15453,10 +15446,10 @@
         <v>422</v>
       </c>
       <c r="F231" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G231" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
@@ -15474,10 +15467,10 @@
         <v>424</v>
       </c>
       <c r="F232" s="19" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G232" s="19" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
@@ -15495,10 +15488,10 @@
         <v>348</v>
       </c>
       <c r="F233" s="21" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="G233" s="21" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
@@ -15632,16 +15625,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
-        <v>976</v>
-      </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
+      <c r="A2" s="83" t="s">
+        <v>975</v>
+      </c>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
       <c r="E2" s="50"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -15665,13 +15658,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -15680,10 +15673,10 @@
         <v>2</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>3</v>
@@ -15695,10 +15688,10 @@
         <v>3</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>8</v>
@@ -15710,10 +15703,10 @@
         <v>4</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>8</v>
@@ -15725,10 +15718,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>8</v>
@@ -15740,10 +15733,10 @@
         <v>6</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>8</v>
@@ -15755,13 +15748,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -15770,10 +15763,10 @@
         <v>8</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="D11" s="21" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>3</v>
@@ -15819,17 +15812,17 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
-        <v>975</v>
-      </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
+      <c r="A2" s="83" t="s">
+        <v>974</v>
+      </c>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -15850,10 +15843,10 @@
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>3</v>
@@ -15863,23 +15856,23 @@
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="14" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="14" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>3</v>
@@ -15889,10 +15882,10 @@
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="49" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>5</v>
@@ -15902,10 +15895,10 @@
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
       <c r="C8" s="14" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>5</v>
@@ -15915,10 +15908,10 @@
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="14" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>5</v>
@@ -15928,10 +15921,10 @@
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
       <c r="C10" s="14" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>5</v>
@@ -15941,23 +15934,23 @@
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="14" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="14" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>167</v>
@@ -15967,65 +15960,65 @@
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="14" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="14" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="14" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
       <c r="C16" s="14" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="20" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="D17" s="21" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -16182,17 +16175,17 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
-        <v>981</v>
-      </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
+      <c r="A2" s="83" t="s">
+        <v>980</v>
+      </c>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -16216,7 +16209,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>3</v>
@@ -16226,26 +16219,26 @@
       <c r="A5" s="13"/>
       <c r="B5" s="13"/>
       <c r="C5" s="14" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
       <c r="B6" s="16"/>
       <c r="C6" s="20" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -16399,425 +16392,425 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="72" t="s">
         <v>593</v>
       </c>
-      <c r="B1" s="80" t="s">
+      <c r="B1" s="72" t="s">
         <v>594</v>
       </c>
-      <c r="C1" s="80" t="s">
+      <c r="C1" s="72" t="s">
+        <v>996</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>595</v>
+      </c>
+      <c r="E1" s="78" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="68" t="s">
         <v>997</v>
       </c>
-      <c r="D1" s="81" t="s">
-        <v>595</v>
-      </c>
-      <c r="E1" s="88" t="s">
+      <c r="B2" s="68">
+        <v>2016</v>
+      </c>
+      <c r="C2" s="70" t="s">
+        <v>596</v>
+      </c>
+      <c r="D2" s="71" t="s">
+        <v>998</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>1019</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
-        <v>998</v>
-      </c>
-      <c r="B2" s="76">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="68"/>
+      <c r="B3" s="68">
         <v>2016</v>
       </c>
-      <c r="C2" s="78" t="s">
-        <v>596</v>
-      </c>
-      <c r="D2" s="79" t="s">
+      <c r="C3" s="70" t="s">
+        <v>597</v>
+      </c>
+      <c r="D3" s="71" t="s">
         <v>999</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>1020</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="76"/>
-      <c r="B3" s="76">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="68"/>
+      <c r="B4" s="68">
         <v>2016</v>
       </c>
-      <c r="C3" s="78" t="s">
-        <v>597</v>
-      </c>
-      <c r="D3" s="79" t="s">
+      <c r="C4" s="70" t="s">
         <v>1000</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="D4" s="71" t="s">
+        <v>1001</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>1021</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="76"/>
-      <c r="B4" s="76">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="68"/>
+      <c r="B5" s="68">
         <v>2016</v>
       </c>
-      <c r="C4" s="78" t="s">
-        <v>1001</v>
-      </c>
-      <c r="D4" s="79" t="s">
+      <c r="C5" s="70" t="s">
         <v>1002</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="D5" s="71" t="s">
+        <v>1003</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="68"/>
+      <c r="B6" s="68">
+        <v>2016</v>
+      </c>
+      <c r="C6" s="70" t="s">
+        <v>598</v>
+      </c>
+      <c r="D6" s="71" t="s">
+        <v>599</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>1022</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="76"/>
-      <c r="B5" s="76">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="68"/>
+      <c r="B7" s="68">
         <v>2016</v>
       </c>
-      <c r="C5" s="78" t="s">
-        <v>1003</v>
-      </c>
-      <c r="D5" s="79" t="s">
+      <c r="C7" s="70" t="s">
+        <v>600</v>
+      </c>
+      <c r="D7" s="71" t="s">
+        <v>601</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>1021</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="68"/>
+      <c r="B8" s="68">
+        <v>2016</v>
+      </c>
+      <c r="C8" s="70" t="s">
+        <v>602</v>
+      </c>
+      <c r="D8" s="71" t="s">
         <v>1004</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>1022</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="76"/>
-      <c r="B6" s="76">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="68"/>
+      <c r="B9" s="68">
         <v>2016</v>
       </c>
-      <c r="C6" s="78" t="s">
-        <v>598</v>
-      </c>
-      <c r="D6" s="79" t="s">
-        <v>599</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="C9" s="70" t="s">
+        <v>603</v>
+      </c>
+      <c r="D9" s="71" t="s">
+        <v>1005</v>
+      </c>
+      <c r="E9" s="74" t="s">
         <v>1023</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="76"/>
-      <c r="B7" s="76">
-        <v>2016</v>
-      </c>
-      <c r="C7" s="78" t="s">
-        <v>600</v>
-      </c>
-      <c r="D7" s="79" t="s">
-        <v>601</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>1022</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="76"/>
-      <c r="B8" s="76">
-        <v>2016</v>
-      </c>
-      <c r="C8" s="78" t="s">
-        <v>602</v>
-      </c>
-      <c r="D8" s="79" t="s">
-        <v>1005</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>1023</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="76"/>
-      <c r="B9" s="76">
-        <v>2016</v>
-      </c>
-      <c r="C9" s="78" t="s">
-        <v>603</v>
-      </c>
-      <c r="D9" s="79" t="s">
+    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="68" t="s">
         <v>1006</v>
       </c>
-      <c r="E9" s="82" t="s">
+      <c r="B10" s="68">
+        <v>2018</v>
+      </c>
+      <c r="C10" s="70" t="s">
+        <v>1007</v>
+      </c>
+      <c r="D10" s="71" t="s">
+        <v>1008</v>
+      </c>
+      <c r="E10" s="74" t="s">
         <v>1024</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="76" t="s">
-        <v>1007</v>
-      </c>
-      <c r="B10" s="76">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="68" t="s">
+        <v>604</v>
+      </c>
+      <c r="B11" s="68"/>
+      <c r="C11" s="70" t="s">
+        <v>1009</v>
+      </c>
+      <c r="D11" s="71"/>
+      <c r="E11" s="74" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="87"/>
+      <c r="B12" s="87">
         <v>2018</v>
       </c>
-      <c r="C10" s="78" t="s">
-        <v>1008</v>
-      </c>
-      <c r="D10" s="79" t="s">
-        <v>1009</v>
-      </c>
-      <c r="E10" s="82" t="s">
+      <c r="C12" s="68" t="s">
+        <v>1010</v>
+      </c>
+      <c r="D12" s="88" t="s">
+        <v>605</v>
+      </c>
+      <c r="E12" s="74"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="87"/>
+      <c r="B13" s="87"/>
+      <c r="C13" s="68" t="s">
+        <v>1011</v>
+      </c>
+      <c r="D13" s="88"/>
+      <c r="E13" s="74"/>
+    </row>
+    <row r="14" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="68"/>
+      <c r="B14" s="68">
+        <v>2018</v>
+      </c>
+      <c r="C14" s="68" t="s">
+        <v>606</v>
+      </c>
+      <c r="D14" s="71" t="s">
+        <v>607</v>
+      </c>
+      <c r="E14" s="74" t="s">
         <v>1025</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="76" t="s">
-        <v>604</v>
-      </c>
-      <c r="B11" s="76"/>
-      <c r="C11" s="78" t="s">
-        <v>1010</v>
-      </c>
-      <c r="D11" s="79"/>
-      <c r="E11" s="82" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="68"/>
+      <c r="B15" s="68">
+        <v>2018</v>
+      </c>
+      <c r="C15" s="68" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D15" s="71" t="s">
+        <v>605</v>
+      </c>
+      <c r="E15" s="74" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="68"/>
+      <c r="B16" s="68">
+        <v>2018</v>
+      </c>
+      <c r="C16" s="68" t="s">
+        <v>1013</v>
+      </c>
+      <c r="D16" s="71" t="s">
+        <v>605</v>
+      </c>
+      <c r="E16" s="74" t="s">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="68" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B17" s="68">
+        <v>2019</v>
+      </c>
+      <c r="C17" s="70" t="s">
+        <v>1015</v>
+      </c>
+      <c r="D17" s="71" t="s">
+        <v>605</v>
+      </c>
+      <c r="E17" s="74" t="s">
         <v>1026</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="77"/>
-      <c r="B12" s="77">
-        <v>2018</v>
-      </c>
-      <c r="C12" s="76" t="s">
-        <v>1011</v>
-      </c>
-      <c r="D12" s="83" t="s">
+    <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="68" t="s">
+        <v>608</v>
+      </c>
+      <c r="B18" s="68">
+        <v>2019</v>
+      </c>
+      <c r="C18" s="70" t="s">
+        <v>609</v>
+      </c>
+      <c r="D18" s="71" t="s">
         <v>605</v>
       </c>
-      <c r="E12" s="82"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="77"/>
-      <c r="B13" s="77"/>
-      <c r="C13" s="76" t="s">
-        <v>1012</v>
-      </c>
-      <c r="D13" s="83"/>
-      <c r="E13" s="82"/>
-    </row>
-    <row r="14" spans="1:5" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="76"/>
-      <c r="B14" s="76">
-        <v>2018</v>
-      </c>
-      <c r="C14" s="76" t="s">
-        <v>606</v>
-      </c>
-      <c r="D14" s="79" t="s">
-        <v>607</v>
-      </c>
-      <c r="E14" s="82" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="76"/>
-      <c r="B15" s="76">
-        <v>2018</v>
-      </c>
-      <c r="C15" s="76" t="s">
-        <v>1013</v>
-      </c>
-      <c r="D15" s="79" t="s">
+      <c r="E18" s="75" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="68" t="s">
+        <v>610</v>
+      </c>
+      <c r="B19" s="68">
+        <v>2017</v>
+      </c>
+      <c r="C19" s="70" t="s">
+        <v>611</v>
+      </c>
+      <c r="D19" s="71" t="s">
         <v>605</v>
       </c>
-      <c r="E15" s="82" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="76"/>
-      <c r="B16" s="76">
-        <v>2018</v>
-      </c>
-      <c r="C16" s="76" t="s">
-        <v>1014</v>
-      </c>
-      <c r="D16" s="79" t="s">
+      <c r="E19" s="75" t="s">
+        <v>1028</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="68" t="s">
+        <v>612</v>
+      </c>
+      <c r="B20" s="68">
+        <v>2017</v>
+      </c>
+      <c r="C20" s="76" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D20" s="71" t="s">
         <v>605</v>
       </c>
-      <c r="E16" s="82" t="s">
-        <v>1026</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="76" t="s">
-        <v>1015</v>
-      </c>
-      <c r="B17" s="76">
-        <v>2019</v>
-      </c>
-      <c r="C17" s="78" t="s">
-        <v>1016</v>
-      </c>
-      <c r="D17" s="79" t="s">
-        <v>605</v>
-      </c>
-      <c r="E17" s="82" t="s">
-        <v>1027</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="76" t="s">
-        <v>608</v>
-      </c>
-      <c r="B18" s="76">
-        <v>2019</v>
-      </c>
-      <c r="C18" s="78" t="s">
-        <v>609</v>
-      </c>
-      <c r="D18" s="79" t="s">
-        <v>605</v>
-      </c>
-      <c r="E18" s="84" t="s">
-        <v>1028</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="76" t="s">
-        <v>610</v>
-      </c>
-      <c r="B19" s="76">
-        <v>2017</v>
-      </c>
-      <c r="C19" s="78" t="s">
-        <v>611</v>
-      </c>
-      <c r="D19" s="79" t="s">
-        <v>605</v>
-      </c>
-      <c r="E19" s="84" t="s">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="74" t="s">
-        <v>612</v>
-      </c>
-      <c r="B20" s="74">
-        <v>2017</v>
-      </c>
-      <c r="C20" s="85" t="s">
+    </row>
+    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="68" t="s">
+        <v>613</v>
+      </c>
+      <c r="B21" s="69" t="s">
+        <v>614</v>
+      </c>
+      <c r="C21" s="68" t="s">
         <v>1017</v>
       </c>
-      <c r="D20" s="86" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="74" t="s">
-        <v>613</v>
-      </c>
-      <c r="B21" s="75" t="s">
-        <v>614</v>
-      </c>
-      <c r="C21" s="74" t="s">
-        <v>1018</v>
-      </c>
-      <c r="D21" s="86" t="s">
+      <c r="D21" s="71" t="s">
         <v>615</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C22" s="32" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="D22" s="23"/>
-      <c r="E22" s="89" t="s">
-        <v>1030</v>
+      <c r="E22" s="79" t="s">
+        <v>1029</v>
       </c>
       <c r="F22" s="23"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C23" s="32" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="D23" s="23"/>
-      <c r="E23" s="90" t="s">
+      <c r="E23" s="23" t="s">
         <v>636</v>
       </c>
       <c r="F23" s="23"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C24" s="32" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="D24" s="23"/>
-      <c r="E24" s="90" t="s">
+      <c r="E24" s="23" t="s">
         <v>637</v>
       </c>
       <c r="F24" s="23"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C25" s="32" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="D25" s="23"/>
-      <c r="E25" s="90" t="s">
+      <c r="E25" s="23" t="s">
         <v>638</v>
       </c>
       <c r="F25" s="23"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C26" s="32" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="D26" s="23"/>
-      <c r="E26" s="90" t="s">
+      <c r="E26" s="23" t="s">
         <v>639</v>
       </c>
       <c r="F26" s="23"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C27" s="32" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="D27" s="23"/>
-      <c r="E27" s="90" t="s">
+      <c r="E27" s="23" t="s">
         <v>640</v>
       </c>
       <c r="F27" s="23"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C28" s="32" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D28" s="23"/>
-      <c r="E28" s="90" t="s">
+      <c r="E28" s="23" t="s">
         <v>641</v>
       </c>
       <c r="F28" s="23"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C29" s="32" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D29" s="23"/>
-      <c r="E29" s="90" t="s">
+      <c r="E29" s="23" t="s">
         <v>642</v>
       </c>
       <c r="F29" s="23"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C30" s="32" t="s">
+        <v>1037</v>
+      </c>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23" t="s">
+        <v>643</v>
+      </c>
+      <c r="F30" s="23"/>
+    </row>
+    <row r="31" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="C31" s="80" t="s">
         <v>1038</v>
       </c>
-      <c r="D30" s="23"/>
-      <c r="E30" s="90" t="s">
-        <v>643</v>
-      </c>
-      <c r="F30" s="23"/>
-    </row>
-    <row r="31" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="C31" s="91" t="s">
+      <c r="D31" s="23"/>
+      <c r="E31" s="23" t="s">
+        <v>644</v>
+      </c>
+      <c r="F31" s="23"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="77"/>
+      <c r="B32" s="77"/>
+      <c r="C32" s="33" t="s">
         <v>1039</v>
-      </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="90" t="s">
-        <v>644</v>
-      </c>
-      <c r="F31" s="23"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="87"/>
-      <c r="B32" s="87"/>
-      <c r="C32" s="33" t="s">
-        <v>1040</v>
       </c>
       <c r="D32" s="24"/>
       <c r="E32" s="24" t="s">

</xml_diff>